<commit_message>
didactic attendance import completed
</commit_message>
<xml_diff>
--- a/backend/0. Personal Details.xlsx
+++ b/backend/0. Personal Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheryl_malfoy/Desktop/Import files for SingHealth Testing/NEW DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63920554-62DE-B74E-8A89-A3F5B8E368C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32949188-0986-384B-A6D3-039825D63686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7220" yWindow="1640" windowWidth="16860" windowHeight="15040" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1700,7 +1700,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="O23" sqref="O23"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>